<commit_message>
Dictionary Engine - global filter
</commit_message>
<xml_diff>
--- a/SchVictorina.WebAPI/Config/countries.xlsx
+++ b/SchVictorina.WebAPI/Config/countries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\schvictorina\schvictorina\SchVictorina.WebAPI\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7E8DBD-DD7F-49AC-8398-C1081E7AD1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D3ED45-5AEB-4E39-89F2-DE6D1A4DA070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{64543D42-3327-43A5-9629-52F4FACA7A12}"/>
+    <workbookView xWindow="3285" yWindow="3270" windowWidth="17250" windowHeight="8865" activeTab="1" xr2:uid="{64543D42-3327-43A5-9629-52F4FACA7A12}"/>
   </bookViews>
   <sheets>
     <sheet name="Данные" sheetId="2" r:id="rId1"/>

</xml_diff>

<commit_message>
Dictionary engine - equal
</commit_message>
<xml_diff>
--- a/SchVictorina.WebAPI/Config/countries.xlsx
+++ b/SchVictorina.WebAPI/Config/countries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\schvictorina\schvictorina\SchVictorina.WebAPI\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D3ED45-5AEB-4E39-89F2-DE6D1A4DA070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3F3A7A-0CD9-4AAC-B24A-B746098C9975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3285" yWindow="3270" windowWidth="17250" windowHeight="8865" activeTab="1" xr2:uid="{64543D42-3327-43A5-9629-52F4FACA7A12}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{64543D42-3327-43A5-9629-52F4FACA7A12}"/>
   </bookViews>
   <sheets>
     <sheet name="Данные" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="610">
   <si>
     <t>Столица</t>
   </si>
@@ -1833,9 +1833,6 @@
   </si>
   <si>
     <t>answer</t>
-  </si>
-  <si>
-    <t>wrongOrderMaxIndex</t>
   </si>
   <si>
     <t>notequal</t>
@@ -2281,18 +2278,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F962963F-E303-48FB-8562-C84169DA6B71}">
   <dimension ref="A1:E198"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>589</v>
       </c>
@@ -2309,7 +2308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>241</v>
       </c>
@@ -2326,7 +2325,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>181</v>
       </c>
@@ -2343,7 +2342,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>467</v>
       </c>
@@ -2360,7 +2359,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>184</v>
       </c>
@@ -2377,7 +2376,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>79</v>
       </c>
@@ -2394,7 +2393,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>371</v>
       </c>
@@ -2411,7 +2410,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>350</v>
       </c>
@@ -2428,7 +2427,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
@@ -2445,7 +2444,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>400</v>
       </c>
@@ -2462,7 +2461,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>586</v>
       </c>
@@ -2479,7 +2478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>321</v>
       </c>
@@ -2496,7 +2495,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>520</v>
       </c>
@@ -2513,7 +2512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>571</v>
       </c>
@@ -2530,7 +2529,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>111</v>
       </c>
@@ -2547,7 +2546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>169</v>
       </c>
@@ -2564,7 +2563,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>166</v>
       </c>
@@ -2581,7 +2580,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>137</v>
       </c>
@@ -2598,7 +2597,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>193</v>
       </c>
@@ -2615,7 +2614,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>499</v>
       </c>
@@ -2632,7 +2631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>476</v>
       </c>
@@ -2649,7 +2648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>99</v>
       </c>
@@ -2666,7 +2665,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>526</v>
       </c>
@@ -2683,7 +2682,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>205</v>
       </c>
@@ -2700,7 +2699,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>574</v>
       </c>
@@ -2717,7 +2716,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>397</v>
       </c>
@@ -2734,7 +2733,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>335</v>
       </c>
@@ -2751,7 +2750,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>479</v>
       </c>
@@ -2768,7 +2767,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>247</v>
       </c>
@@ -2785,7 +2784,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>202</v>
       </c>
@@ -2802,7 +2801,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>229</v>
       </c>
@@ -2819,7 +2818,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
@@ -2836,7 +2835,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>508</v>
       </c>
@@ -2853,7 +2852,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>461</v>
       </c>
@@ -2870,7 +2869,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>20</v>
       </c>
@@ -2887,7 +2886,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>388</v>
       </c>
@@ -2904,7 +2903,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>190</v>
       </c>
@@ -2921,7 +2920,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>502</v>
       </c>
@@ -2938,7 +2937,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>223</v>
       </c>
@@ -2955,7 +2954,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>315</v>
       </c>
@@ -2972,7 +2971,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>505</v>
       </c>
@@ -2989,7 +2988,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>303</v>
       </c>
@@ -3006,7 +3005,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>385</v>
       </c>
@@ -3023,7 +3022,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>105</v>
       </c>
@@ -3040,7 +3039,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>420</v>
       </c>
@@ -3057,7 +3056,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>40</v>
       </c>
@@ -3074,7 +3073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>344</v>
       </c>
@@ -3091,7 +3090,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>126</v>
       </c>
@@ -3108,7 +3107,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>208</v>
       </c>
@@ -3125,7 +3124,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>324</v>
       </c>
@@ -3142,7 +3141,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>23</v>
       </c>
@@ -3159,7 +3158,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>244</v>
       </c>
@@ -3176,7 +3175,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>297</v>
       </c>
@@ -3193,7 +3192,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>6</v>
       </c>
@@ -3210,7 +3209,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>220</v>
       </c>
@@ -3227,7 +3226,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>256</v>
       </c>
@@ -3244,7 +3243,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>553</v>
       </c>
@@ -3261,7 +3260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>347</v>
       </c>
@@ -3278,7 +3277,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>406</v>
       </c>
@@ -3295,7 +3294,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>85</v>
       </c>
@@ -3312,7 +3311,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>306</v>
       </c>
@@ -3329,7 +3328,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>544</v>
       </c>
@@ -3346,7 +3345,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>214</v>
       </c>
@@ -3363,7 +3362,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>300</v>
       </c>
@@ -3380,7 +3379,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>446</v>
       </c>
@@ -3397,7 +3396,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>353</v>
       </c>
@@ -3414,7 +3413,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>172</v>
       </c>
@@ -3431,7 +3430,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>556</v>
       </c>
@@ -3448,7 +3447,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>129</v>
       </c>
@@ -3465,7 +3464,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>175</v>
       </c>
@@ -3482,7 +3481,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>217</v>
       </c>
@@ -3499,7 +3498,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>429</v>
       </c>
@@ -3516,7 +3515,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>535</v>
       </c>
@@ -3533,7 +3532,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>580</v>
       </c>
@@ -3550,7 +3549,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>458</v>
       </c>
@@ -3567,7 +3566,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>403</v>
       </c>
@@ -3584,7 +3583,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>61</v>
       </c>
@@ -3601,7 +3600,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>259</v>
       </c>
@@ -3618,7 +3617,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>64</v>
       </c>
@@ -3635,7 +3634,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>494</v>
       </c>
@@ -3652,7 +3651,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>88</v>
       </c>
@@ -3669,7 +3668,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>70</v>
       </c>
@@ -3686,7 +3685,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>117</v>
       </c>
@@ -3703,7 +3702,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>149</v>
       </c>
@@ -3720,7 +3719,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>131</v>
       </c>
@@ -3737,7 +3736,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>541</v>
       </c>
@@ -3754,7 +3753,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>391</v>
       </c>
@@ -3771,7 +3770,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>163</v>
       </c>
@@ -3788,7 +3787,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>550</v>
       </c>
@@ -3805,7 +3804,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>441</v>
       </c>
@@ -3822,7 +3821,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>102</v>
       </c>
@@ -3839,7 +3838,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>187</v>
       </c>
@@ -3856,7 +3855,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>14</v>
       </c>
@@ -3873,7 +3872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>58</v>
       </c>
@@ -3890,7 +3889,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>365</v>
       </c>
@@ -3907,7 +3906,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>10</v>
       </c>
@@ -3924,7 +3923,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>140</v>
       </c>
@@ -3941,7 +3940,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>178</v>
       </c>
@@ -3958,7 +3957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>473</v>
       </c>
@@ -3975,7 +3974,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>547</v>
       </c>
@@ -3992,7 +3991,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>379</v>
       </c>
@@ -4009,7 +4008,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>67</v>
       </c>
@@ -4026,7 +4025,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>482</v>
       </c>
@@ -4043,7 +4042,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>470</v>
       </c>
@@ -4060,7 +4059,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>382</v>
       </c>
@@ -4077,7 +4076,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>265</v>
       </c>
@@ -4094,7 +4093,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>409</v>
       </c>
@@ -4111,7 +4110,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>356</v>
       </c>
@@ -4128,7 +4127,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>280</v>
       </c>
@@ -4145,7 +4144,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>235</v>
       </c>
@@ -4162,7 +4161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>277</v>
       </c>
@@ -4179,7 +4178,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>155</v>
       </c>
@@ -4196,7 +4195,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>444</v>
       </c>
@@ -4213,7 +4212,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>523</v>
       </c>
@@ -4230,7 +4229,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>496</v>
       </c>
@@ -4247,7 +4246,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>449</v>
       </c>
@@ -4264,7 +4263,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>562</v>
       </c>
@@ -4281,7 +4280,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>532</v>
       </c>
@@ -4298,7 +4297,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>362</v>
       </c>
@@ -4315,7 +4314,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>253</v>
       </c>
@@ -4332,7 +4331,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>143</v>
       </c>
@@ -4349,7 +4348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>394</v>
       </c>
@@ -4366,7 +4365,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>359</v>
       </c>
@@ -4383,7 +4382,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>196</v>
       </c>
@@ -4400,7 +4399,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>368</v>
       </c>
@@ -4417,7 +4416,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>262</v>
       </c>
@@ -4434,7 +4433,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>529</v>
       </c>
@@ -4451,7 +4450,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>377</v>
       </c>
@@ -4468,7 +4467,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>274</v>
       </c>
@@ -4485,7 +4484,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>73</v>
       </c>
@@ -4502,7 +4501,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>152</v>
       </c>
@@ -4519,7 +4518,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>327</v>
       </c>
@@ -4536,7 +4535,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>294</v>
       </c>
@@ -4553,7 +4552,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>511</v>
       </c>
@@ -4570,7 +4569,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>332</v>
       </c>
@@ -4587,7 +4586,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>37</v>
       </c>
@@ -4604,7 +4603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>283</v>
       </c>
@@ -4621,7 +4620,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>17</v>
       </c>
@@ -4638,7 +4637,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>583</v>
       </c>
@@ -4655,7 +4654,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>226</v>
       </c>
@@ -4672,7 +4671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>338</v>
       </c>
@@ -4689,7 +4688,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>76</v>
       </c>
@@ -4706,7 +4705,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>271</v>
       </c>
@@ -4723,7 +4722,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>423</v>
       </c>
@@ -4740,7 +4739,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>452</v>
       </c>
@@ -4757,7 +4756,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>123</v>
       </c>
@@ -4774,7 +4773,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>268</v>
       </c>
@@ -4791,7 +4790,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>114</v>
       </c>
@@ -4808,7 +4807,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>134</v>
       </c>
@@ -4825,7 +4824,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>565</v>
       </c>
@@ -4842,7 +4841,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>52</v>
       </c>
@@ -4859,7 +4858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>488</v>
       </c>
@@ -4876,7 +4875,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>568</v>
       </c>
@@ -4893,7 +4892,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>291</v>
       </c>
@@ -4910,7 +4909,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>559</v>
       </c>
@@ -4927,7 +4926,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>108</v>
       </c>
@@ -4944,7 +4943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>517</v>
       </c>
@@ -4961,7 +4960,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>158</v>
       </c>
@@ -4978,7 +4977,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>232</v>
       </c>
@@ -4995,7 +4994,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>250</v>
       </c>
@@ -5012,7 +5011,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>91</v>
       </c>
@@ -5029,7 +5028,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>120</v>
       </c>
@@ -5046,7 +5045,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>455</v>
       </c>
@@ -5063,7 +5062,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>538</v>
       </c>
@@ -5080,7 +5079,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>289</v>
       </c>
@@ -5097,7 +5096,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>464</v>
       </c>
@@ -5114,7 +5113,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>211</v>
       </c>
@@ -5131,7 +5130,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>82</v>
       </c>
@@ -5148,7 +5147,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>312</v>
       </c>
@@ -5165,7 +5164,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>309</v>
       </c>
@@ -5182,7 +5181,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>43</v>
       </c>
@@ -5199,7 +5198,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>55</v>
       </c>
@@ -5216,7 +5215,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>199</v>
       </c>
@@ -5233,7 +5232,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>49</v>
       </c>
@@ -5250,7 +5249,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>94</v>
       </c>
@@ -5267,7 +5266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>2</v>
       </c>
@@ -5284,7 +5283,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>412</v>
       </c>
@@ -5301,7 +5300,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>417</v>
       </c>
@@ -5318,7 +5317,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>438</v>
       </c>
@@ -5335,7 +5334,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>146</v>
       </c>
@@ -5352,7 +5351,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>432</v>
       </c>
@@ -5369,7 +5368,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>238</v>
       </c>
@@ -5386,7 +5385,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>485</v>
       </c>
@@ -5403,7 +5402,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>514</v>
       </c>
@@ -5420,7 +5419,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>29</v>
       </c>
@@ -5437,7 +5436,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>426</v>
       </c>
@@ -5454,7 +5453,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>26</v>
       </c>
@@ -5471,7 +5470,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>160</v>
       </c>
@@ -5488,7 +5487,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>318</v>
       </c>
@@ -5505,7 +5504,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>577</v>
       </c>
@@ -5522,7 +5521,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>435</v>
       </c>
@@ -5539,7 +5538,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>330</v>
       </c>
@@ -5556,7 +5555,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>286</v>
       </c>
@@ -5573,7 +5572,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>415</v>
       </c>
@@ -5590,7 +5589,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>374</v>
       </c>
@@ -5607,7 +5606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>341</v>
       </c>
@@ -5624,7 +5623,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>491</v>
       </c>
@@ -5641,7 +5640,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>97</v>
       </c>
@@ -5668,24 +5667,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD99A6B-D1F7-4689-9959-BE6147912039}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" customWidth="1"/>
-    <col min="3" max="4" width="15.88671875" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="63.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>593</v>
       </c>
@@ -5699,7 +5697,7 @@
         <v>595</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>596</v>
@@ -5707,13 +5705,10 @@
       <c r="G1" s="2" t="s">
         <v>597</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E2" t="s">
         <v>590</v>
@@ -5721,21 +5716,18 @@
       <c r="F2" t="s">
         <v>589</v>
       </c>
-      <c r="G2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F3" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -5744,9 +5736,9 @@
         <v>589</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -5755,9 +5747,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -5768,13 +5760,10 @@
       <c r="F6" t="s">
         <v>589</v>
       </c>
-      <c r="G6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
@@ -5785,52 +5774,49 @@
       <c r="F7" t="s">
         <v>589</v>
       </c>
-      <c r="G7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F8" t="s">
         <v>1</v>
       </c>
-      <c r="H8" t="s">
+      <c r="G8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F9" t="s">
         <v>1</v>
       </c>
-      <c r="H9" t="s">
+      <c r="G9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B10" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F10" t="s">
         <v>589</v>
       </c>
-      <c r="H10" t="s">
+      <c r="G10" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>606</v>
+      </c>
+      <c r="B11" t="s">
         <v>607</v>
-      </c>
-      <c r="B11" t="s">
-        <v>608</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
bug fixing and small features
</commit_message>
<xml_diff>
--- a/SchVictorina.WebAPI/Config/countries.xlsx
+++ b/SchVictorina.WebAPI/Config/countries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\schvictorina\schvictorina\SchVictorina.WebAPI\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA43691-0691-4D84-9CE4-601EF741081A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7D0517-BB2E-464B-95E5-8C7F831AE876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{64543D42-3327-43A5-9629-52F4FACA7A12}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{64543D42-3327-43A5-9629-52F4FACA7A12}"/>
   </bookViews>
   <sheets>
     <sheet name="Данные" sheetId="2" r:id="rId1"/>
@@ -1244,9 +1244,6 @@
     <t>Какая страна с населением {Население} человек?</t>
   </si>
   <si>
-    <t>Какая страна с населением {Население} в {Континент}</t>
-  </si>
-  <si>
     <t>Население &gt; 100 000 000</t>
   </si>
   <si>
@@ -1869,6 +1866,9 @@
   </si>
   <si>
     <t>[нет столицы]</t>
+  </si>
+  <si>
+    <t>Какая страна с населением {Население} человек в части света {Континент}?</t>
   </si>
 </sst>
 </file>
@@ -2276,20 +2276,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F962963F-E303-48FB-8562-C84169DA6B71}">
   <dimension ref="A1:E198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="B200" sqref="B200"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>384</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>158</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>159</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D2" s="2">
         <v>1410549741</v>
@@ -2323,7 +2323,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>118</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>119</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D3" s="2">
         <v>1268961000</v>
@@ -2340,7 +2340,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>305</v>
       </c>
@@ -2348,16 +2348,16 @@
         <v>306</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D4" s="2">
         <v>322762018</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>120</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>121</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D5" s="2">
         <v>255461700</v>
@@ -2374,7 +2374,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>53</v>
       </c>
@@ -2382,16 +2382,16 @@
         <v>54</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D6" s="2">
         <v>206081432</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>245</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>246</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D7" s="2">
         <v>196174380</v>
@@ -2408,7 +2408,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>232</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>233</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D8" s="2">
         <v>186988000</v>
@@ -2425,7 +2425,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>31</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D9" s="2">
         <v>160221000</v>
@@ -2442,7 +2442,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>262</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>263</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D10" s="2">
         <v>146267288</v>
@@ -2459,7 +2459,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>382</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>383</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D11" s="2">
         <v>127103388</v>
@@ -2476,7 +2476,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>212</v>
       </c>
@@ -2484,16 +2484,16 @@
         <v>213</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D12" s="2">
         <v>122273473</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>341</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>342</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D13" s="2">
         <v>102980480</v>
@@ -2510,7 +2510,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>374</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>375</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D14" s="2">
         <v>101853000</v>
@@ -2527,7 +2527,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>74</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>75</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D15" s="2">
         <v>91713300</v>
@@ -2544,7 +2544,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>110</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>111</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D16" s="2">
         <v>91701723</v>
@@ -2561,15 +2561,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>109</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D17" s="2">
         <v>85026000</v>
@@ -2578,7 +2578,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>91</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>92</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D18" s="2">
         <v>82175684</v>
@@ -2595,7 +2595,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>126</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>127</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D19" s="2">
         <v>80840713</v>
@@ -2612,7 +2612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>327</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>328</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D20" s="2">
         <v>78741053</v>
@@ -2629,7 +2629,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>311</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>312</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D21" s="2">
         <v>68147000</v>
@@ -2646,7 +2646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>67</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>68</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D22" s="2">
         <v>65341183</v>
@@ -2663,7 +2663,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>345</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>346</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D23" s="2">
         <v>64513242</v>
@@ -2680,7 +2680,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>134</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>135</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D24" s="2">
         <v>60665551</v>
@@ -2697,7 +2697,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>376</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>377</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D25" s="2">
         <v>55908900</v>
@@ -2714,15 +2714,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>261</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D26" s="2">
         <v>51664244</v>
@@ -2731,7 +2731,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>222</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>223</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D27" s="2">
         <v>51419420</v>
@@ -2748,7 +2748,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>313</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>314</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D28" s="2">
         <v>50142938</v>
@@ -2765,7 +2765,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>162</v>
       </c>
@@ -2773,16 +2773,16 @@
         <v>163</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D29" s="2">
         <v>48892070</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>132</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>133</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D30" s="2">
         <v>46438422</v>
@@ -2799,7 +2799,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>150</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>151</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D31" s="2">
         <v>44156577</v>
@@ -2816,7 +2816,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>23</v>
       </c>
@@ -2824,16 +2824,16 @@
         <v>24</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D32" s="2">
         <v>43847000</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>333</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>334</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D33" s="2">
         <v>42650186</v>
@@ -2850,7 +2850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>301</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>302</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D34" s="2">
         <v>41176000</v>
@@ -2867,7 +2867,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>14</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>14</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D35" s="2">
         <v>39813722</v>
@@ -2884,7 +2884,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>256</v>
       </c>
@@ -2892,7 +2892,7 @@
         <v>257</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D36" s="2">
         <v>37967209</v>
@@ -2901,7 +2901,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>124</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>125</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D37" s="2">
         <v>37883543</v>
@@ -2918,7 +2918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>329</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>330</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D38" s="2">
         <v>36860700</v>
@@ -2935,7 +2935,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>146</v>
       </c>
@@ -2943,16 +2943,16 @@
         <v>147</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D39" s="2">
         <v>36286425</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>208</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>209</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D40" s="2">
         <v>34817000</v>
@@ -2969,7 +2969,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>331</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>332</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D41" s="2">
         <v>31807000</v>
@@ -2986,7 +2986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>199</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>200</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D42" s="2">
         <v>31790277</v>
@@ -3003,7 +3003,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>254</v>
       </c>
@@ -3011,16 +3011,16 @@
         <v>255</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D43" s="2">
         <v>31488625</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>71</v>
       </c>
@@ -3028,24 +3028,24 @@
         <v>72</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D44" s="2">
         <v>31028637</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>275</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D45" s="2">
         <v>31015999</v>
@@ -3054,7 +3054,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>27</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>28</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D46" s="2">
         <v>29822848</v>
@@ -3071,7 +3071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>228</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>229</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D47" s="2">
         <v>28431494</v>
@@ -3088,7 +3088,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>84</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>85</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D48" s="2">
         <v>28308301</v>
@@ -3105,7 +3105,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>136</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>137</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D49" s="2">
         <v>27478000</v>
@@ -3122,7 +3122,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>214</v>
       </c>
@@ -3130,7 +3130,7 @@
         <v>215</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D50" s="2">
         <v>26423623</v>
@@ -3139,7 +3139,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>16</v>
       </c>
@@ -3147,7 +3147,7 @@
         <v>17</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D51" s="2">
         <v>25831000</v>
@@ -3156,7 +3156,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>160</v>
       </c>
@@ -3164,7 +3164,7 @@
         <v>161</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D52" s="2">
         <v>25281000</v>
@@ -3173,7 +3173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>195</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>196</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D53" s="2">
         <v>24430325</v>
@@ -3190,7 +3190,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>5</v>
       </c>
@@ -3198,16 +3198,16 @@
         <v>6</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D54" s="2">
         <v>24238610</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>144</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>145</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D55" s="2">
         <v>23924000</v>
@@ -3224,7 +3224,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>167</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>168</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D56" s="2">
         <v>23254000</v>
@@ -3241,7 +3241,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>363</v>
       </c>
@@ -3249,7 +3249,7 @@
         <v>364</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D57" s="2">
         <v>21866445</v>
@@ -3258,7 +3258,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>230</v>
       </c>
@@ -3266,7 +3266,7 @@
         <v>231</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D58" s="2">
         <v>20715000</v>
@@ -3275,7 +3275,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>266</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>267</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D59" s="2">
         <v>19759968</v>
@@ -3292,7 +3292,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>57</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>58</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D60" s="2">
         <v>19034397</v>
@@ -3309,7 +3309,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>201</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>202</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D61" s="2">
         <v>18135000</v>
@@ -3326,7 +3326,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>357</v>
       </c>
@@ -3334,16 +3334,16 @@
         <v>358</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D62" s="2">
         <v>18006407</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>140</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>141</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D63" s="2">
         <v>17753200</v>
@@ -3360,7 +3360,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>197</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>198</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D64" s="2">
         <v>17377468</v>
@@ -3377,7 +3377,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>292</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>293</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D65" s="2">
         <v>17185170</v>
@@ -3394,7 +3394,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>234</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>235</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D66" s="2">
         <v>16979120</v>
@@ -3411,7 +3411,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>112</v>
       </c>
@@ -3419,7 +3419,7 @@
         <v>113</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D67" s="2">
         <v>16717000</v>
@@ -3428,7 +3428,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>365</v>
       </c>
@@ -3436,16 +3436,16 @@
         <v>366</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D68" s="2">
         <v>16599593</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>86</v>
       </c>
@@ -3453,16 +3453,16 @@
         <v>86</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D69" s="2">
         <v>16555556</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>114</v>
       </c>
@@ -3470,7 +3470,7 @@
         <v>115</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D70" s="2">
         <v>15967000</v>
@@ -3479,7 +3479,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>142</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>143</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D71" s="2">
         <v>15827000</v>
@@ -3496,7 +3496,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>279</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v>280</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D72" s="2">
         <v>14799859</v>
@@ -3513,7 +3513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>351</v>
       </c>
@@ -3521,7 +3521,7 @@
         <v>352</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D73" s="2">
         <v>14497000</v>
@@ -3530,15 +3530,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>379</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D74" s="2">
         <v>12733000</v>
@@ -3547,7 +3547,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>299</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>300</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D75" s="2">
         <v>12316895</v>
@@ -3564,7 +3564,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>264</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>265</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D76" s="2">
         <v>11533446</v>
@@ -3581,7 +3581,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>42</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>43</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D77" s="2">
         <v>11250585</v>
@@ -3598,7 +3598,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>169</v>
       </c>
@@ -3606,16 +3606,16 @@
         <v>170</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D78" s="2">
         <v>11236348</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>44</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>45</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D79" s="2">
         <v>11167000</v>
@@ -3632,7 +3632,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>324</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>324</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D80" s="2">
         <v>11154372</v>
@@ -3649,7 +3649,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>59</v>
       </c>
@@ -3657,7 +3657,7 @@
         <v>60</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D81" s="2">
         <v>11099298</v>
@@ -3666,7 +3666,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>48</v>
       </c>
@@ -3674,16 +3674,16 @@
         <v>49</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D82" s="2">
         <v>10985059</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>78</v>
       </c>
@@ -3691,16 +3691,16 @@
         <v>79</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D83" s="2">
         <v>10911819</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>98</v>
       </c>
@@ -3708,7 +3708,7 @@
         <v>99</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D84" s="2">
         <v>10793526</v>
@@ -3717,7 +3717,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>87</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>88</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D85" s="2">
         <v>10628972</v>
@@ -3734,7 +3734,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>355</v>
       </c>
@@ -3742,7 +3742,7 @@
         <v>356</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D86" s="2">
         <v>10553843</v>
@@ -3751,7 +3751,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>258</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>259</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D87" s="2">
         <v>10341330</v>
@@ -3768,24 +3768,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>108</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D88" s="2">
         <v>10075045</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>361</v>
       </c>
@@ -3793,7 +3793,7 @@
         <v>362</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D89" s="2">
         <v>9851017</v>
@@ -3802,7 +3802,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>288</v>
       </c>
@@ -3810,7 +3810,7 @@
         <v>289</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D90" s="2">
         <v>9846582</v>
@@ -3819,7 +3819,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>69</v>
       </c>
@@ -3827,7 +3827,7 @@
         <v>70</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D91" s="2">
         <v>9830485</v>
@@ -3836,7 +3836,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>122</v>
       </c>
@@ -3844,7 +3844,7 @@
         <v>123</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D92" s="2">
         <v>9813095</v>
@@ -3853,7 +3853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>10</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>11</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D93" s="2">
         <v>9705600</v>
@@ -3870,7 +3870,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>40</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>41</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D94" s="2">
         <v>9498400</v>
@@ -3887,7 +3887,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>241</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>242</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D95" s="2">
         <v>9267000</v>
@@ -3904,7 +3904,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>7</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>8</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D96" s="2">
         <v>8741753</v>
@@ -3921,7 +3921,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
         <v>93</v>
       </c>
@@ -3929,16 +3929,16 @@
         <v>94</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D97" s="2">
         <v>8721014</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
         <v>116</v>
       </c>
@@ -3946,7 +3946,7 @@
         <v>117</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D98" s="2">
         <v>8585000</v>
@@ -3955,7 +3955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
         <v>309</v>
       </c>
@@ -3963,7 +3963,7 @@
         <v>310</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D99" s="2">
         <v>8551000</v>
@@ -3972,7 +3972,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
         <v>359</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>360</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D100" s="2">
         <v>8325194</v>
@@ -3989,24 +3989,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>251</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D101" s="2">
         <v>8151300</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
         <v>46</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>47</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D102" s="2">
         <v>7153784</v>
@@ -4023,7 +4023,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
         <v>315</v>
       </c>
@@ -4031,7 +4031,7 @@
         <v>316</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D103" s="2">
         <v>7143000</v>
@@ -4040,7 +4040,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>307</v>
       </c>
@@ -4048,7 +4048,7 @@
         <v>308</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D104" s="2">
         <v>7075641</v>
@@ -4057,7 +4057,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
         <v>252</v>
       </c>
@@ -4065,16 +4065,16 @@
         <v>253</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D105" s="2">
         <v>6854536</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
         <v>173</v>
       </c>
@@ -4082,7 +4082,7 @@
         <v>174</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D106" s="2">
         <v>6492400</v>
@@ -4091,7 +4091,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
         <v>268</v>
       </c>
@@ -4099,16 +4099,16 @@
         <v>269</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D107" s="2">
         <v>6460271</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>236</v>
       </c>
@@ -4116,16 +4116,16 @@
         <v>237</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D108" s="2">
         <v>6262703</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>183</v>
       </c>
@@ -4133,7 +4133,7 @@
         <v>184</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D109" s="2">
         <v>6244174</v>
@@ -4142,7 +4142,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
         <v>154</v>
       </c>
@@ -4150,7 +4150,7 @@
         <v>155</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D110" s="2">
         <v>6019500</v>
@@ -4159,7 +4159,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
         <v>181</v>
       </c>
@@ -4167,7 +4167,7 @@
         <v>182</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D111" s="2">
         <v>5988000</v>
@@ -4176,7 +4176,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
         <v>102</v>
       </c>
@@ -4184,7 +4184,7 @@
         <v>103</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D112" s="2">
         <v>5707251</v>
@@ -4193,7 +4193,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
         <v>290</v>
       </c>
@@ -4210,7 +4210,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
         <v>343</v>
       </c>
@@ -4218,7 +4218,7 @@
         <v>344</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D114" s="2">
         <v>5487308</v>
@@ -4227,7 +4227,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
         <v>325</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>326</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D115" s="2">
         <v>5439000</v>
@@ -4244,7 +4244,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
         <v>294</v>
       </c>
@@ -4252,7 +4252,7 @@
         <v>295</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D116" s="2">
         <v>5426252</v>
@@ -4261,7 +4261,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
         <v>368</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>369</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D117" s="2">
         <v>5352000</v>
@@ -4278,7 +4278,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
         <v>349</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>350</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D118" s="2">
         <v>5277959</v>
@@ -4295,7 +4295,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
         <v>239</v>
       </c>
@@ -4303,7 +4303,7 @@
         <v>240</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D119" s="2">
         <v>5213985</v>
@@ -4312,7 +4312,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
         <v>165</v>
       </c>
@@ -4320,24 +4320,24 @@
         <v>166</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D120" s="2">
         <v>4890379</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="B121" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="C121" s="3" t="s">
         <v>532</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>533</v>
       </c>
       <c r="D121" s="2">
         <v>4816503</v>
@@ -4346,15 +4346,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>260</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D122" s="2">
         <v>4741000</v>
@@ -4363,24 +4363,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>238</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D123" s="2">
         <v>4722321</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
         <v>128</v>
       </c>
@@ -4388,7 +4388,7 @@
         <v>129</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D124" s="2">
         <v>4658530</v>
@@ -4397,7 +4397,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
         <v>243</v>
       </c>
@@ -4405,7 +4405,7 @@
         <v>244</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D125" s="2">
         <v>4523401</v>
@@ -4414,7 +4414,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
         <v>171</v>
       </c>
@@ -4422,7 +4422,7 @@
         <v>172</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D126" s="2">
         <v>4330308</v>
@@ -4431,7 +4431,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
         <v>347</v>
       </c>
@@ -4439,7 +4439,7 @@
         <v>348</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D127" s="2">
         <v>4190669</v>
@@ -4448,7 +4448,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
         <v>250</v>
       </c>
@@ -4456,16 +4456,16 @@
         <v>250</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D128" s="2">
         <v>4037043</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
         <v>179</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>180</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D129" s="2">
         <v>4001855</v>
@@ -4482,15 +4482,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D130" s="2">
         <v>3802000</v>
@@ -4499,7 +4499,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
         <v>100</v>
       </c>
@@ -4507,7 +4507,7 @@
         <v>101</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D131" s="2">
         <v>3720400</v>
@@ -4516,7 +4516,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
         <v>216</v>
       </c>
@@ -4524,7 +4524,7 @@
         <v>217</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D132" s="2">
         <v>3553056</v>
@@ -4533,7 +4533,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
         <v>193</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>194</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D133" s="2">
         <v>3537368</v>
@@ -4550,7 +4550,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
         <v>335</v>
       </c>
@@ -4558,16 +4558,16 @@
         <v>336</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D134" s="2">
         <v>3480222</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
         <v>220</v>
       </c>
@@ -4575,7 +4575,7 @@
         <v>221</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D135" s="2">
         <v>3081677</v>
@@ -4584,7 +4584,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
         <v>25</v>
       </c>
@@ -4592,7 +4592,7 @@
         <v>26</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D136" s="2">
         <v>2995100</v>
@@ -4601,7 +4601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
         <v>185</v>
       </c>
@@ -4609,7 +4609,7 @@
         <v>186</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D137" s="2">
         <v>2888558</v>
@@ -4618,7 +4618,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
         <v>12</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>13</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D138" s="2">
         <v>2866026</v>
@@ -4635,7 +4635,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
         <v>380</v>
       </c>
@@ -4643,16 +4643,16 @@
         <v>381</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D139" s="2">
         <v>2723000</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
         <v>148</v>
       </c>
@@ -4660,7 +4660,7 @@
         <v>149</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D140" s="2">
         <v>2553393</v>
@@ -4669,7 +4669,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
         <v>224</v>
       </c>
@@ -4677,7 +4677,7 @@
         <v>225</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D141" s="2">
         <v>2436469</v>
@@ -4686,7 +4686,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
         <v>51</v>
       </c>
@@ -4694,7 +4694,7 @@
         <v>52</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D142" s="2">
         <v>2209208</v>
@@ -4703,7 +4703,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
         <v>177</v>
       </c>
@@ -4711,7 +4711,7 @@
         <v>178</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D143" s="2">
         <v>2160000</v>
@@ -4720,15 +4720,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>276</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D144" s="2">
         <v>2071278</v>
@@ -4737,7 +4737,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
         <v>296</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>297</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D145" s="2">
         <v>2064188</v>
@@ -4754,7 +4754,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="s">
         <v>82</v>
       </c>
@@ -4762,7 +4762,7 @@
         <v>83</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D146" s="2">
         <v>2025527</v>
@@ -4771,7 +4771,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="s">
         <v>175</v>
       </c>
@@ -4779,7 +4779,7 @@
         <v>176</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D147" s="2">
         <v>1968957</v>
@@ -4788,7 +4788,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
         <v>76</v>
       </c>
@@ -4796,7 +4796,7 @@
         <v>77</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D148" s="2">
         <v>1811079</v>
@@ -4805,7 +4805,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="s">
         <v>89</v>
       </c>
@@ -4813,7 +4813,7 @@
         <v>90</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D149" s="2">
         <v>1547754</v>
@@ -4822,7 +4822,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="s">
         <v>370</v>
       </c>
@@ -4830,7 +4830,7 @@
         <v>371</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D150" s="2">
         <v>1419623</v>
@@ -4839,7 +4839,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="s">
         <v>35</v>
       </c>
@@ -4856,24 +4856,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B152" s="3" t="s">
         <v>320</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D152" s="2">
         <v>1349667</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="3" t="s">
         <v>372</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>373</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D153" s="2">
         <v>1315944</v>
@@ -4890,7 +4890,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" s="3" t="s">
         <v>191</v>
       </c>
@@ -4898,7 +4898,7 @@
         <v>192</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D154" s="2">
         <v>1263747</v>
@@ -4907,15 +4907,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B155" s="3" t="s">
         <v>367</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D155" s="2">
         <v>1222442</v>
@@ -4924,15 +4924,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B156" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D156" s="2">
         <v>1167242</v>
@@ -4941,7 +4941,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" s="3" t="s">
         <v>339</v>
       </c>
@@ -4949,16 +4949,16 @@
         <v>340</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D157" s="2">
         <v>903207</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
         <v>104</v>
       </c>
@@ -4966,7 +4966,7 @@
         <v>104</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D158" s="2">
         <v>890179</v>
@@ -4975,7 +4975,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" s="3" t="s">
         <v>152</v>
       </c>
@@ -4983,7 +4983,7 @@
         <v>153</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D159" s="2">
         <v>848319</v>
@@ -4992,15 +4992,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="3" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B160" s="3" t="s">
         <v>164</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D160" s="2">
         <v>806153</v>
@@ -5009,7 +5009,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="3" t="s">
         <v>61</v>
       </c>
@@ -5017,7 +5017,7 @@
         <v>62</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D161" s="2">
         <v>784000</v>
@@ -5026,7 +5026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="3" t="s">
         <v>80</v>
       </c>
@@ -5034,33 +5034,33 @@
         <v>81</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D162" s="2">
         <v>741962</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B163" s="3" t="s">
         <v>298</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D163" s="2">
         <v>651700</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" s="3" t="s">
         <v>353</v>
       </c>
@@ -5068,7 +5068,7 @@
         <v>354</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D164" s="2">
         <v>622218</v>
@@ -5077,7 +5077,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="3" t="s">
         <v>190</v>
       </c>
@@ -5085,7 +5085,7 @@
         <v>190</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D165" s="2">
         <v>576249</v>
@@ -5094,7 +5094,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="3" t="s">
         <v>303</v>
       </c>
@@ -5102,16 +5102,16 @@
         <v>304</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D166" s="2">
         <v>558773</v>
       </c>
       <c r="E166" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="3" t="s">
         <v>138</v>
       </c>
@@ -5119,7 +5119,7 @@
         <v>139</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D167" s="2">
         <v>538535</v>
@@ -5128,7 +5128,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="3" t="s">
         <v>55</v>
       </c>
@@ -5136,7 +5136,7 @@
         <v>56</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D168" s="2">
         <v>436620</v>
@@ -5145,7 +5145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="3" t="s">
         <v>205</v>
       </c>
@@ -5162,9 +5162,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B170" s="3" t="s">
         <v>203</v>
@@ -5179,24 +5179,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B171" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D171" s="2">
         <v>393000</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="3" t="s">
         <v>38</v>
       </c>
@@ -5204,16 +5204,16 @@
         <v>39</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D172" s="2">
         <v>377968</v>
       </c>
       <c r="E172" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" s="3" t="s">
         <v>130</v>
       </c>
@@ -5221,7 +5221,7 @@
         <v>131</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D173" s="2">
         <v>332529</v>
@@ -5230,7 +5230,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="3" t="s">
         <v>32</v>
       </c>
@@ -5244,10 +5244,10 @@
         <v>291495</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="3" t="s">
         <v>63</v>
       </c>
@@ -5255,16 +5255,16 @@
         <v>64</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D175" s="2">
         <v>289700</v>
       </c>
       <c r="E175" s="3" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="3" t="s">
         <v>2</v>
       </c>
@@ -5272,7 +5272,7 @@
         <v>3</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D176" s="2">
         <v>243564</v>
@@ -5281,7 +5281,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="3" t="s">
         <v>270</v>
       </c>
@@ -5289,24 +5289,24 @@
         <v>271</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D177" s="2">
         <v>194899</v>
       </c>
       <c r="E177" s="3" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B178" s="3" t="s">
         <v>274</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D178" s="2">
         <v>194000</v>
@@ -5315,7 +5315,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="3" t="s">
         <v>285</v>
       </c>
@@ -5329,10 +5329,10 @@
         <v>172818</v>
       </c>
       <c r="E179" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="3" t="s">
         <v>95</v>
       </c>
@@ -5346,12 +5346,12 @@
         <v>110566</v>
       </c>
       <c r="E180" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B181" s="3" t="s">
         <v>281</v>
@@ -5363,15 +5363,15 @@
         <v>110255</v>
       </c>
       <c r="E181" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" s="3" t="s">
         <v>156</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C182" s="3" t="s">
         <v>157</v>
@@ -5380,10 +5380,10 @@
         <v>109693</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="3" t="s">
         <v>317</v>
       </c>
@@ -5397,12 +5397,12 @@
         <v>106440</v>
       </c>
       <c r="E183" s="3" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B184" s="3" t="s">
         <v>337</v>
@@ -5414,12 +5414,12 @@
         <v>105681</v>
       </c>
       <c r="E184" s="3" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B185" s="3" t="s">
         <v>21</v>
@@ -5431,12 +5431,12 @@
         <v>93581</v>
       </c>
       <c r="E185" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B186" s="3" t="s">
         <v>277</v>
@@ -5451,7 +5451,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="3" t="s">
         <v>18</v>
       </c>
@@ -5468,7 +5468,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="3" t="s">
         <v>105</v>
       </c>
@@ -5482,12 +5482,12 @@
         <v>69393</v>
       </c>
       <c r="E188" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B189" s="3" t="s">
         <v>210</v>
@@ -5499,18 +5499,18 @@
         <v>55717</v>
       </c>
       <c r="E189" s="3" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B190" s="3" t="s">
         <v>378</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D190" s="2">
         <v>53532</v>
@@ -5519,9 +5519,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B191" s="3" t="s">
         <v>283</v>
@@ -5533,10 +5533,10 @@
         <v>52329</v>
       </c>
       <c r="E191" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" s="3" t="s">
         <v>218</v>
       </c>
@@ -5553,7 +5553,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="3" t="s">
         <v>187</v>
       </c>
@@ -5570,7 +5570,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="3" t="s">
         <v>272</v>
       </c>
@@ -5587,7 +5587,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="3" t="s">
         <v>247</v>
       </c>
@@ -5601,15 +5601,15 @@
         <v>17661</v>
       </c>
       <c r="E195" s="3" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" s="3" t="s">
         <v>226</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C196" s="3" t="s">
         <v>227</v>
@@ -5618,10 +5618,10 @@
         <v>10800</v>
       </c>
       <c r="E196" s="3" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" s="3" t="s">
         <v>321</v>
       </c>
@@ -5635,10 +5635,10 @@
         <v>10782</v>
       </c>
       <c r="E197" s="3" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" s="3" t="s">
         <v>65</v>
       </c>
@@ -5667,20 +5667,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD99A6B-D1F7-4689-9959-BE6147912039}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="63.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="63.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="3" max="4" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>388</v>
       </c>
@@ -5694,15 +5694,15 @@
         <v>390</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E2" t="s">
         <v>385</v>
@@ -5711,7 +5711,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>392</v>
       </c>
@@ -5719,7 +5719,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>392</v>
       </c>
@@ -5730,7 +5730,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>393</v>
       </c>
@@ -5741,7 +5741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>394</v>
       </c>
@@ -5755,7 +5755,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>395</v>
       </c>
@@ -5769,7 +5769,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>396</v>
       </c>
@@ -5777,7 +5777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>397</v>
       </c>
@@ -5785,7 +5785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>399</v>
       </c>
@@ -5796,12 +5796,12 @@
         <v>384</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>608</v>
+      </c>
+      <c r="B11" t="s">
         <v>400</v>
-      </c>
-      <c r="B11" t="s">
-        <v>401</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>

</xml_diff>